<commit_message>
Concentrator TX-RX by timeout, low precision due to int ms
</commit_message>
<xml_diff>
--- a/Armlet/Armlet3/Armlet3_hw/Gerber/Armlet3_BOM.xlsx
+++ b/Armlet/Armlet3/Armlet3_hw/Gerber/Armlet3_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="11565"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="21840" windowHeight="11565"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="152">
   <si>
     <t>DA1</t>
   </si>
@@ -63,9 +63,6 @@
     <t>QFN20</t>
   </si>
   <si>
-    <t>CC1101</t>
-  </si>
-  <si>
     <t>DD2</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>QFN16_5</t>
   </si>
   <si>
-    <t>MMA8452Q</t>
-  </si>
-  <si>
     <t>Q4</t>
   </si>
   <si>
@@ -243,9 +237,6 @@
     <t>R18</t>
   </si>
   <si>
-    <t>47R</t>
-  </si>
-  <si>
     <t>R20, R25</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>R14</t>
   </si>
   <si>
-    <t>200R</t>
-  </si>
-  <si>
     <t>R7, R9, R37</t>
   </si>
   <si>
@@ -420,9 +408,6 @@
     <t>C24, C26, C27, C31, C35, C41, C50</t>
   </si>
   <si>
-    <t>Armlet_BOM v.20130324.1912</t>
-  </si>
-  <si>
     <t>LCD 24@0.4</t>
   </si>
   <si>
@@ -469,6 +454,24 @@
   </si>
   <si>
     <t>Предоставим в ленте</t>
+  </si>
+  <si>
+    <t>Solder Point per cmp</t>
+  </si>
+  <si>
+    <t>SolderPoint total</t>
+  </si>
+  <si>
+    <t>Solder points per brd</t>
+  </si>
+  <si>
+    <t>51R</t>
+  </si>
+  <si>
+    <t>Armlet_BOM v.20130328.2012</t>
+  </si>
+  <si>
+    <t>220R</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -557,6 +560,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -564,7 +593,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -613,6 +642,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
@@ -917,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,42 +961,50 @@
     <col min="3" max="3" width="20.140625" style="14" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="F2" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>121</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -990,15 +1029,22 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="F5">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <f>F5*D5</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>7</v>
@@ -1007,10 +1053,17 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G68" si="0">F6*D6</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1024,10 +1077,17 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1041,832 +1101,1248 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="B14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="B15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B19" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>35</v>
-      </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="B24" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C24" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="B26" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B29" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="14" t="s">
+      <c r="B33" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>145</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="14" t="s">
+      <c r="B34" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="14" t="s">
+      <c r="B36" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="D36">
         <v>27</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D37">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="14" t="s">
+      <c r="C39" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="D39">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>145</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="B42" s="14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="C42" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="B43" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="C43" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>145</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="B44" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="B45" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B46" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="14" t="s">
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>145</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B47" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="14" t="s">
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="D48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>85</v>
       </c>
       <c r="D50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D51">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>145</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>145</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="14" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>145</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B54" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>145</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="14" t="s">
+      <c r="B55" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>95</v>
       </c>
       <c r="D55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="14" t="s">
         <v>96</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D58">
         <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>145</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="14" t="s">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>145</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="B61" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
         <v>104</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="16"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>145</v>
+      </c>
+      <c r="F63">
+        <v>28</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C63" s="14" t="s">
+      <c r="B66" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>145</v>
+      </c>
+      <c r="F66">
+        <v>12</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>145</v>
+      </c>
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>140</v>
-      </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F69" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G69" s="21">
+        <f>SUM(G4:G68)</f>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>